<commit_message>
fixed taxi TP, added taxi and first edition over years
</commit_message>
<xml_diff>
--- a/xlsx/Taxi-docF-redig.xlsx
+++ b/xlsx/Taxi-docF-redig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsaules\Github\lnb_transports\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A16B2ED-2F90-4CAF-A095-569146B3C621}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF8692A-CFA9-4397-9DDC-2F27E397E7F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10395" activeTab="1" xr2:uid="{A642A053-A12A-4A70-BEA5-507B6F07D2F3}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1873,9 +1873,6 @@
     <t>PavlA</t>
   </si>
   <si>
-    <t>Celop</t>
-  </si>
-  <si>
     <t>PerlL</t>
   </si>
   <si>
@@ -1918,9 +1915,6 @@
     <t>SkujF</t>
   </si>
   <si>
-    <t>SirdS</t>
-  </si>
-  <si>
     <t>SpriJ</t>
   </si>
   <si>
@@ -2063,6 +2057,12 @@
   </si>
   <si>
     <t>PrusE</t>
+  </si>
+  <si>
+    <t>CeloP</t>
+  </si>
+  <si>
+    <t>SidrS</t>
   </si>
 </sst>
 </file>
@@ -4687,7 +4687,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB53342C-5C34-4DB4-B5A0-C93BF7D4ADCC}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB53342C-5C34-4DB4-B5A0-C93BF7D4ADCC}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -5154,19 +5154,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B1" t="s">
+        <v>667</v>
+      </c>
+      <c r="C1" t="s">
+        <v>662</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1" t="s">
         <v>670</v>
-      </c>
-      <c r="B1" t="s">
-        <v>669</v>
-      </c>
-      <c r="C1" t="s">
-        <v>664</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>671</v>
-      </c>
-      <c r="E1" t="s">
-        <v>672</v>
       </c>
       <c r="F1" t="s">
         <v>359</v>
@@ -11384,8 +11384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C535F9-1ECA-42B4-8749-D7A8591B5E63}">
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="G164" sqref="G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11395,16 +11395,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>565</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11871,10 +11871,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C35" s="7">
         <v>1936</v>
@@ -13386,7 +13386,7 @@
         <v>609</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>610</v>
+        <v>672</v>
       </c>
       <c r="C143" s="6">
         <v>1939</v>
@@ -13397,10 +13397,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B144" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C144" s="7">
         <v>1937</v>
@@ -13411,10 +13411,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B145" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C145" s="6">
         <v>1937</v>
@@ -13425,10 +13425,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B146" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C146" s="7">
         <v>1937</v>
@@ -13439,10 +13439,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B147" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B147" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C147" s="6">
         <v>1937</v>
@@ -13453,10 +13453,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B148" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B148" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C148" s="7">
         <v>1937</v>
@@ -13467,10 +13467,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B149" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C149" s="6">
         <v>1937</v>
@@ -13481,10 +13481,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B150" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B150" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C150" s="7">
         <v>1937</v>
@@ -13495,10 +13495,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B151" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B151" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C151" s="6">
         <v>1937</v>
@@ -13509,10 +13509,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B152" s="7" t="s">
         <v>611</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="C152" s="7">
         <v>1937</v>
@@ -13523,10 +13523,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="B153" s="6" t="s">
         <v>613</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>614</v>
       </c>
       <c r="C153" s="6">
         <v>1935</v>
@@ -13537,10 +13537,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="B154" s="6" t="s">
         <v>616</v>
-      </c>
-      <c r="B154" s="6" t="s">
-        <v>617</v>
       </c>
       <c r="C154" s="6">
         <v>1938</v>
@@ -13551,10 +13551,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="B155" s="6" t="s">
         <v>616</v>
-      </c>
-      <c r="B155" s="6" t="s">
-        <v>617</v>
       </c>
       <c r="C155" s="7">
         <v>1938</v>
@@ -13565,10 +13565,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B156" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>619</v>
       </c>
       <c r="C156" s="6">
         <v>1928</v>
@@ -13579,10 +13579,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B157" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B157" s="6" t="s">
-        <v>619</v>
       </c>
       <c r="C157" s="7">
         <v>1928</v>
@@ -13593,10 +13593,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B158" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>619</v>
       </c>
       <c r="C158" s="6">
         <v>1928</v>
@@ -13607,10 +13607,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B159" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B159" s="6" t="s">
-        <v>619</v>
       </c>
       <c r="C159" s="7">
         <v>1928</v>
@@ -13621,10 +13621,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B160" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>619</v>
       </c>
       <c r="C160" s="6">
         <v>1928</v>
@@ -13635,10 +13635,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="B161" s="7" t="s">
         <v>620</v>
-      </c>
-      <c r="B161" s="7" t="s">
-        <v>621</v>
       </c>
       <c r="C161" s="7">
         <v>1932</v>
@@ -13649,10 +13649,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>620</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>621</v>
       </c>
       <c r="C162" s="6">
         <v>1932</v>
@@ -13663,10 +13663,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="B163" s="7" t="s">
         <v>622</v>
-      </c>
-      <c r="B163" s="7" t="s">
-        <v>623</v>
       </c>
       <c r="C163" s="7">
         <v>1936</v>
@@ -13677,10 +13677,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>625</v>
+        <v>673</v>
       </c>
       <c r="C164" s="6">
         <v>1924</v>
@@ -13691,10 +13691,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>625</v>
+        <v>673</v>
       </c>
       <c r="C165" s="7">
         <v>1924</v>
@@ -13705,10 +13705,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>625</v>
+        <v>673</v>
       </c>
       <c r="C166" s="6">
         <v>1924</v>
@@ -13719,10 +13719,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="B167" s="6" t="s">
         <v>626</v>
-      </c>
-      <c r="B167" s="6" t="s">
-        <v>628</v>
       </c>
       <c r="C167" s="6">
         <v>1929</v>
@@ -13733,10 +13733,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="B168" s="6" t="s">
         <v>626</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>628</v>
       </c>
       <c r="C168" s="7">
         <v>1929</v>
@@ -13747,10 +13747,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="B169" s="6" t="s">
         <v>626</v>
-      </c>
-      <c r="B169" s="6" t="s">
-        <v>628</v>
       </c>
       <c r="C169" s="6">
         <v>1929</v>
@@ -13761,10 +13761,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="B170" s="6" t="s">
         <v>626</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>628</v>
       </c>
       <c r="C170" s="7">
         <v>1929</v>
@@ -13775,10 +13775,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="B171" s="6" t="s">
         <v>626</v>
-      </c>
-      <c r="B171" s="6" t="s">
-        <v>628</v>
       </c>
       <c r="C171" s="6">
         <v>1929</v>
@@ -13789,10 +13789,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="9" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C172" s="7">
         <v>1939</v>
@@ -13803,10 +13803,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C173" s="7">
         <v>1932</v>
@@ -13817,7 +13817,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B174" s="6" t="s">
         <v>605</v>
@@ -13831,7 +13831,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>605</v>
@@ -13845,7 +13845,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>605</v>
@@ -13859,7 +13859,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>605</v>
@@ -13873,10 +13873,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C178" s="6">
         <v>1937</v>
@@ -13887,10 +13887,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C179" s="7">
         <v>1937</v>
@@ -13901,10 +13901,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="8" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C180" s="6">
         <v>1930</v>
@@ -13915,10 +13915,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="8" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C181" s="7">
         <v>1930</v>
@@ -13929,10 +13929,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="9" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C182" s="7">
         <v>1926</v>
@@ -13943,10 +13943,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C183" s="6">
         <v>1932</v>
@@ -13957,10 +13957,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C184" s="6">
         <v>1937</v>
@@ -13971,10 +13971,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="B185" s="7" t="s">
         <v>635</v>
-      </c>
-      <c r="B185" s="7" t="s">
-        <v>637</v>
       </c>
       <c r="C185" s="7">
         <v>1939</v>
@@ -13985,10 +13985,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="B186" s="7" t="s">
         <v>635</v>
-      </c>
-      <c r="B186" s="7" t="s">
-        <v>637</v>
       </c>
       <c r="C186" s="6">
         <v>1939</v>
@@ -13999,10 +13999,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C187" s="7">
         <v>1936</v>
@@ -14013,10 +14013,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C188" s="6">
         <v>1936</v>
@@ -14027,10 +14027,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C189" s="7">
         <v>1936</v>
@@ -14041,10 +14041,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C190" s="6">
         <v>1936</v>
@@ -14055,10 +14055,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C191" s="7">
         <v>1936</v>
@@ -14069,10 +14069,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B192" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B192" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C192" s="7">
         <v>1931</v>
@@ -14083,10 +14083,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B193" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B193" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C193" s="6">
         <v>1931</v>
@@ -14097,10 +14097,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B194" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B194" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C194" s="7">
         <v>1931</v>
@@ -14111,10 +14111,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B195" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B195" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C195" s="6">
         <v>1931</v>
@@ -14125,10 +14125,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B196" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B196" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C196" s="7">
         <v>1931</v>
@@ -14139,10 +14139,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B197" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B197" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C197" s="6">
         <v>1931</v>
@@ -14153,10 +14153,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B198" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B198" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C198" s="7">
         <v>1931</v>
@@ -14167,10 +14167,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B199" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="B199" s="7" t="s">
-        <v>644</v>
       </c>
       <c r="C199" s="6">
         <v>1931</v>
@@ -14181,10 +14181,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C200" s="6">
         <v>1934</v>
@@ -14195,10 +14195,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="9" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C201" s="7">
         <v>1931</v>
@@ -14209,10 +14209,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="9" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C202" s="6">
         <v>1931</v>
@@ -14223,10 +14223,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C203" s="7">
         <v>1927</v>
@@ -14237,10 +14237,10 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C204" s="6">
         <v>1927</v>
@@ -14251,10 +14251,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="9" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C205" s="7">
         <v>1932</v>
@@ -14265,10 +14265,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C206" s="6">
         <v>1928</v>
@@ -14279,10 +14279,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C207" s="7">
         <v>1928</v>
@@ -14293,10 +14293,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C208" s="6">
         <v>1928</v>
@@ -14307,10 +14307,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C209" s="7">
         <v>1928</v>
@@ -14321,10 +14321,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C210" s="6">
         <v>1928</v>
@@ -14335,10 +14335,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B211" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="B211" s="7" t="s">
-        <v>653</v>
       </c>
       <c r="C211" s="7">
         <v>1929</v>
@@ -14349,10 +14349,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B212" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="B212" s="7" t="s">
-        <v>653</v>
       </c>
       <c r="C212" s="6">
         <v>1929</v>
@@ -14363,10 +14363,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B213" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="B213" s="7" t="s">
-        <v>653</v>
       </c>
       <c r="C213" s="7">
         <v>1929</v>
@@ -14377,10 +14377,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B214" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="B214" s="7" t="s">
-        <v>653</v>
       </c>
       <c r="C214" s="6">
         <v>1929</v>
@@ -14391,10 +14391,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B215" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="B215" s="7" t="s">
-        <v>653</v>
       </c>
       <c r="C215" s="7">
         <v>1929</v>
@@ -14405,10 +14405,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C216" s="6">
         <v>1940</v>
@@ -14419,10 +14419,10 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C217" s="7">
         <v>1940</v>
@@ -14433,10 +14433,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C218" s="6">
         <v>1940</v>
@@ -14447,10 +14447,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="9" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C219" s="7">
         <v>1939</v>
@@ -14461,10 +14461,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C220" s="6">
         <v>1931</v>
@@ -14475,10 +14475,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C221" s="7">
         <v>1931</v>
@@ -14489,10 +14489,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C222" s="6">
         <v>1931</v>
@@ -14503,10 +14503,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="9" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C223" s="6">
         <v>1931</v>
@@ -14517,10 +14517,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="9" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C224" s="7">
         <v>1931</v>
@@ -14531,10 +14531,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="9" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C225" s="6">
         <v>1931</v>
@@ -14545,10 +14545,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="9" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C226" s="7">
         <v>1933</v>
@@ -14559,10 +14559,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="B227" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="B227" s="6" t="s">
-        <v>661</v>
       </c>
       <c r="C227" s="6">
         <v>1933</v>
@@ -14573,10 +14573,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="B228" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="B228" s="6" t="s">
-        <v>661</v>
       </c>
       <c r="C228" s="7">
         <v>1933</v>
@@ -14587,10 +14587,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="B229" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="B229" s="6" t="s">
-        <v>661</v>
       </c>
       <c r="C229" s="6">
         <v>1933</v>
@@ -14601,10 +14601,10 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="B230" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="B230" s="6" t="s">
-        <v>661</v>
       </c>
       <c r="C230" s="7">
         <v>1933</v>
@@ -14615,10 +14615,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="B231" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="B231" s="6" t="s">
-        <v>661</v>
       </c>
       <c r="C231" s="6">
         <v>1933</v>
@@ -14629,10 +14629,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="B232" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="B232" s="6" t="s">
-        <v>661</v>
       </c>
       <c r="C232" s="7">
         <v>1933</v>
@@ -14665,10 +14665,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="B3" t="s">
         <v>666</v>
-      </c>
-      <c r="B3" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -14809,7 +14809,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B21" s="16">
         <v>231</v>

</xml_diff>